<commit_message>
More data added, more simulations tidied
</commit_message>
<xml_diff>
--- a/Prototypes/Barley/Observations/MCPD10_11Water.xlsx
+++ b/Prototypes/Barley/Observations/MCPD10_11Water.xlsx
@@ -59,28 +59,28 @@
     <t>ProfileWater</t>
   </si>
   <si>
-    <t>MCPD10_11_Booma</t>
+    <t>MCPD10_11CultBooma</t>
   </si>
   <si>
-    <t>MCPD10_11_County</t>
+    <t>MCPD10_11CultCounty</t>
   </si>
   <si>
-    <t>MCPD10_11_Dash</t>
+    <t>MCPD10_11CultDash</t>
   </si>
   <si>
-    <t>MCPD10_11_Hooded</t>
+    <t>MCPD10_11CultHooded</t>
   </si>
   <si>
-    <t>MCPD10_11_Omaka</t>
+    <t>MCPD10_11CultOmaka</t>
   </si>
   <si>
-    <t>MCPD10_11_Optic</t>
+    <t>MCPD10_11CultOptic</t>
   </si>
   <si>
-    <t>MCPD10_11_Quench</t>
+    <t>MCPD10_11CultQuench</t>
   </si>
   <si>
-    <t>MCPD10_11_Retriever</t>
+    <t>MCPD10_11CultRetriever</t>
   </si>
 </sst>
 </file>
@@ -405,11 +405,12 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection sqref="A1:A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>